<commit_message>
Modul 4 Membuat Model dengan Hyper Parameter Tunning
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7210"/>
+    <workbookView windowWidth="18530" windowHeight="7270"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>Task</t>
   </si>
@@ -70,23 +70,27 @@
     <t>-</t>
   </si>
   <si>
-    <t>Tahap Fitting</t>
-  </si>
-  <si>
     <t xml:space="preserve">Membuat Model CNN 2 dengan Batch Normalization dan DropOut </t>
+  </si>
+  <si>
+    <t>Membuat Model 1 CNN dengan Hyperparameter tuning</t>
+  </si>
+  <si>
+    <t>Membuat Model 2 CNN dengan Hyperparameter tuning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="d\ mmmm\ yyyy"/>
+  <numFmts count="7">
+    <numFmt numFmtId="176" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="177" formatCode="dd\-mmm"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="181" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="181" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="182" formatCode="d\ mmmm\ yyyy"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -113,9 +117,31 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -127,24 +153,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -205,8 +224,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
@@ -214,51 +262,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -285,43 +289,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,43 +457,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -382,90 +470,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -518,6 +522,36 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -572,6 +606,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -580,194 +623,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -775,13 +779,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -790,13 +794,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1060,16 +1067,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="71.6636363636364" customWidth="1"/>
-    <col min="2" max="2" width="21.8636363636364" customWidth="1"/>
+    <col min="2" max="2" width="15.8909090909091" customWidth="1"/>
     <col min="3" max="3" width="20.7090909090909" customWidth="1"/>
     <col min="4" max="4" width="20.2909090909091" customWidth="1"/>
     <col min="5" max="5" width="21.7090909090909" customWidth="1"/>
@@ -1233,12 +1240,12 @@
         <v>7</v>
       </c>
       <c r="F8" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" spans="1:6">
+      <c r="A9" s="9" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="9" customHeight="1" spans="1:5">
-      <c r="A9" s="9" t="s">
-        <v>19</v>
       </c>
       <c r="B9" s="8">
         <v>44477</v>
@@ -1252,6 +1259,57 @@
       <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
+      <c r="F9" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" spans="1:6">
+      <c r="A10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="11">
+        <v>44529</v>
+      </c>
+      <c r="C10" s="10">
+        <v>44530</v>
+      </c>
+      <c r="D10" s="10">
+        <v>44530</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" customHeight="1" spans="1:6">
+      <c r="A11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="11">
+        <v>44529</v>
+      </c>
+      <c r="C11" s="10">
+        <v>44530</v>
+      </c>
+      <c r="D11" s="10">
+        <v>44530</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" customHeight="1" spans="1:6">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>